<commit_message>
Updated with the new dataset
</commit_message>
<xml_diff>
--- a/Data/Working Data Raw (Testing).xlsx
+++ b/Data/Working Data Raw (Testing).xlsx
@@ -353,8 +353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC341"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AE9" sqref="AE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,7 +543,7 @@
         <v>1851</v>
       </c>
       <c r="AC2">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.2">
@@ -810,7 +810,7 @@
         <v>74171</v>
       </c>
       <c r="AC5">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.2">
@@ -899,7 +899,7 @@
         <v>2998</v>
       </c>
       <c r="AC6">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.2">
@@ -988,7 +988,7 @@
         <v>29955</v>
       </c>
       <c r="AC7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.2">
@@ -1077,7 +1077,7 @@
         <v>1997</v>
       </c>
       <c r="AC8">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.2">
@@ -1166,7 +1166,7 @@
         <v>5838</v>
       </c>
       <c r="AC9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.2">
@@ -1344,7 +1344,7 @@
         <v>6460</v>
       </c>
       <c r="AC11">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.2">
@@ -1522,7 +1522,7 @@
         <v>2042</v>
       </c>
       <c r="AC13">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.2">
@@ -1611,7 +1611,7 @@
         <v>1255</v>
       </c>
       <c r="AC14">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.2">
@@ -1700,7 +1700,7 @@
         <v>22392</v>
       </c>
       <c r="AC15">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.2">
@@ -1789,7 +1789,7 @@
         <v>299357</v>
       </c>
       <c r="AC16">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.2">
@@ -1878,7 +1878,7 @@
         <v>1339</v>
       </c>
       <c r="AC17">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.2">
@@ -1967,7 +1967,7 @@
         <v>101337</v>
       </c>
       <c r="AC18">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.2">
@@ -2056,7 +2056,7 @@
         <v>28295</v>
       </c>
       <c r="AC19">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.2">
@@ -2145,7 +2145,7 @@
         <v>2701</v>
       </c>
       <c r="AC20">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.2">
@@ -2234,7 +2234,7 @@
         <v>650</v>
       </c>
       <c r="AC21">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.2">
@@ -2323,7 +2323,7 @@
         <v>13386</v>
       </c>
       <c r="AC22">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.2">
@@ -2412,7 +2412,7 @@
         <v>848</v>
       </c>
       <c r="AC23">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.2">
@@ -2501,7 +2501,7 @@
         <v>4981</v>
       </c>
       <c r="AC24">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.2">
@@ -2590,7 +2590,7 @@
         <v>852</v>
       </c>
       <c r="AC25">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:29" x14ac:dyDescent="0.2">
@@ -2679,7 +2679,7 @@
         <v>720</v>
       </c>
       <c r="AC26">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.2">
@@ -2768,7 +2768,7 @@
         <v>64252</v>
       </c>
       <c r="AC27">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:29" x14ac:dyDescent="0.2">
@@ -2857,7 +2857,7 @@
         <v>5557</v>
       </c>
       <c r="AC28">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:29" x14ac:dyDescent="0.2">
@@ -2946,7 +2946,7 @@
         <v>693</v>
       </c>
       <c r="AC29">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.2">
@@ -3035,7 +3035,7 @@
         <v>1834</v>
       </c>
       <c r="AC30">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
@@ -3213,7 +3213,7 @@
         <v>1215941</v>
       </c>
       <c r="AC32">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.2">
@@ -3302,7 +3302,7 @@
         <v>12443</v>
       </c>
       <c r="AC33">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:29" x14ac:dyDescent="0.2">
@@ -3391,7 +3391,7 @@
         <v>137561</v>
       </c>
       <c r="AC34">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:29" x14ac:dyDescent="0.2">
@@ -3480,7 +3480,7 @@
         <v>434</v>
       </c>
       <c r="AC35">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:29" x14ac:dyDescent="0.2">
@@ -3569,7 +3569,7 @@
         <v>134748</v>
       </c>
       <c r="AC36">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.2">
@@ -3658,7 +3658,7 @@
         <v>2601</v>
       </c>
       <c r="AC37">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.2">
@@ -3747,7 +3747,7 @@
         <v>6455</v>
       </c>
       <c r="AC38">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
@@ -3925,7 +3925,7 @@
         <v>8589</v>
       </c>
       <c r="AC40">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.2">
@@ -4014,7 +4014,7 @@
         <v>1111</v>
       </c>
       <c r="AC41">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:29" x14ac:dyDescent="0.2">
@@ -4103,7 +4103,7 @@
         <v>1539</v>
       </c>
       <c r="AC42">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.2">
@@ -4281,7 +4281,7 @@
         <v>6072</v>
       </c>
       <c r="AC44">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.2">
@@ -4370,7 +4370,7 @@
         <v>17679</v>
       </c>
       <c r="AC45">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:29" x14ac:dyDescent="0.2">
@@ -4459,7 +4459,7 @@
         <v>1684785</v>
       </c>
       <c r="AC46">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:29" x14ac:dyDescent="0.2">
@@ -4548,7 +4548,7 @@
         <v>27351</v>
       </c>
       <c r="AC47">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:29" x14ac:dyDescent="0.2">
@@ -4637,7 +4637,7 @@
         <v>471</v>
       </c>
       <c r="AC48">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.2">
@@ -4815,7 +4815,7 @@
         <v>8201</v>
       </c>
       <c r="AC50">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.2">
@@ -4904,7 +4904,7 @@
         <v>2477</v>
       </c>
       <c r="AC51">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.2">
@@ -4993,7 +4993,7 @@
         <v>7521</v>
       </c>
       <c r="AC52">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.2">
@@ -5082,7 +5082,7 @@
         <v>7682</v>
       </c>
       <c r="AC53">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:29" x14ac:dyDescent="0.2">
@@ -5171,7 +5171,7 @@
         <v>636</v>
       </c>
       <c r="AC54">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:29" x14ac:dyDescent="0.2">
@@ -5260,7 +5260,7 @@
         <v>323988</v>
       </c>
       <c r="AC55">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:29" x14ac:dyDescent="0.2">
@@ -5349,7 +5349,7 @@
         <v>37213</v>
       </c>
       <c r="AC56">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:29" x14ac:dyDescent="0.2">
@@ -5438,7 +5438,7 @@
         <v>2444</v>
       </c>
       <c r="AC57">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:29" x14ac:dyDescent="0.2">
@@ -5527,7 +5527,7 @@
         <v>1676</v>
       </c>
       <c r="AC58">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:29" x14ac:dyDescent="0.2">
@@ -5705,7 +5705,7 @@
         <v>1542</v>
       </c>
       <c r="AC60">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:29" x14ac:dyDescent="0.2">
@@ -5794,7 +5794,7 @@
         <v>1142461</v>
       </c>
       <c r="AC61">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:29" x14ac:dyDescent="0.2">
@@ -5883,7 +5883,7 @@
         <v>1522</v>
       </c>
       <c r="AC62">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:29" x14ac:dyDescent="0.2">
@@ -5972,7 +5972,7 @@
         <v>4968</v>
       </c>
       <c r="AC63">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.2">
@@ -6061,7 +6061,7 @@
         <v>1743</v>
       </c>
       <c r="AC64">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:29" x14ac:dyDescent="0.2">
@@ -6150,7 +6150,7 @@
         <v>117411</v>
       </c>
       <c r="AC65">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:29" x14ac:dyDescent="0.2">
@@ -6239,7 +6239,7 @@
         <v>910953</v>
       </c>
       <c r="AC66">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:29" x14ac:dyDescent="0.2">
@@ -6328,7 +6328,7 @@
         <v>10682</v>
       </c>
       <c r="AC67">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:29" x14ac:dyDescent="0.2">
@@ -6417,7 +6417,7 @@
         <v>2139</v>
       </c>
       <c r="AC68">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:29" x14ac:dyDescent="0.2">
@@ -6506,7 +6506,7 @@
         <v>1326</v>
       </c>
       <c r="AC69">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:29" x14ac:dyDescent="0.2">
@@ -6595,7 +6595,7 @@
         <v>2072</v>
       </c>
       <c r="AC70">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:29" x14ac:dyDescent="0.2">
@@ -6684,7 +6684,7 @@
         <v>1976</v>
       </c>
       <c r="AC71">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:29" x14ac:dyDescent="0.2">
@@ -6773,7 +6773,7 @@
         <v>1176842</v>
       </c>
       <c r="AC72">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:29" x14ac:dyDescent="0.2">
@@ -6951,7 +6951,7 @@
         <v>5452</v>
       </c>
       <c r="AC74">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:29" x14ac:dyDescent="0.2">
@@ -7129,7 +7129,7 @@
         <v>5909</v>
       </c>
       <c r="AC76">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:29" x14ac:dyDescent="0.2">
@@ -7218,7 +7218,7 @@
         <v>891</v>
       </c>
       <c r="AC77">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:29" x14ac:dyDescent="0.2">
@@ -7396,7 +7396,7 @@
         <v>62657</v>
       </c>
       <c r="AC79">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:29" x14ac:dyDescent="0.2">
@@ -7574,7 +7574,7 @@
         <v>4186</v>
       </c>
       <c r="AC81">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:29" x14ac:dyDescent="0.2">
@@ -7663,7 +7663,7 @@
         <v>5540</v>
       </c>
       <c r="AC82">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:29" x14ac:dyDescent="0.2">
@@ -7752,7 +7752,7 @@
         <v>98172</v>
       </c>
       <c r="AC83">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:29" x14ac:dyDescent="0.2">
@@ -7841,7 +7841,7 @@
         <v>30184</v>
       </c>
       <c r="AC84">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:29" x14ac:dyDescent="0.2">
@@ -7930,7 +7930,7 @@
         <v>13897</v>
       </c>
       <c r="AC85">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:29" x14ac:dyDescent="0.2">
@@ -8019,7 +8019,7 @@
         <v>11046</v>
       </c>
       <c r="AC86">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:29" x14ac:dyDescent="0.2">
@@ -8108,7 +8108,7 @@
         <v>18462</v>
       </c>
       <c r="AC87">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:29" x14ac:dyDescent="0.2">
@@ -8197,7 +8197,7 @@
         <v>654</v>
       </c>
       <c r="AC88">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:29" x14ac:dyDescent="0.2">
@@ -8286,7 +8286,7 @@
         <v>508604</v>
       </c>
       <c r="AC89">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:29" x14ac:dyDescent="0.2">
@@ -8375,7 +8375,7 @@
         <v>12832</v>
       </c>
       <c r="AC90">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:29" x14ac:dyDescent="0.2">
@@ -8464,7 +8464,7 @@
         <v>831</v>
       </c>
       <c r="AC91">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:29" x14ac:dyDescent="0.2">
@@ -8553,7 +8553,7 @@
         <v>28379</v>
       </c>
       <c r="AC92">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:29" x14ac:dyDescent="0.2">
@@ -8731,7 +8731,7 @@
         <v>11412</v>
       </c>
       <c r="AC94">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="1:29" x14ac:dyDescent="0.2">
@@ -8820,7 +8820,7 @@
         <v>190765</v>
       </c>
       <c r="AC95">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:29" x14ac:dyDescent="0.2">
@@ -8909,7 +8909,7 @@
         <v>5008</v>
       </c>
       <c r="AC96">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:29" x14ac:dyDescent="0.2">
@@ -8998,7 +8998,7 @@
         <v>16734</v>
       </c>
       <c r="AC97">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:29" x14ac:dyDescent="0.2">
@@ -9087,7 +9087,7 @@
         <v>2006</v>
       </c>
       <c r="AC98">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:29" x14ac:dyDescent="0.2">
@@ -9176,7 +9176,7 @@
         <v>148098</v>
       </c>
       <c r="AC99">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="1:29" x14ac:dyDescent="0.2">
@@ -9265,7 +9265,7 @@
         <v>2479</v>
       </c>
       <c r="AC100">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="101" spans="1:29" x14ac:dyDescent="0.2">
@@ -9354,7 +9354,7 @@
         <v>2098</v>
       </c>
       <c r="AC101">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="102" spans="1:29" x14ac:dyDescent="0.2">
@@ -9443,7 +9443,7 @@
         <v>68925</v>
       </c>
       <c r="AC102">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:29" x14ac:dyDescent="0.2">
@@ -9532,7 +9532,7 @@
         <v>25463</v>
       </c>
       <c r="AC103">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="1:29" x14ac:dyDescent="0.2">
@@ -9710,7 +9710,7 @@
         <v>1867</v>
       </c>
       <c r="AC105">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="106" spans="1:29" x14ac:dyDescent="0.2">
@@ -9799,7 +9799,7 @@
         <v>3209</v>
       </c>
       <c r="AC106">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:29" x14ac:dyDescent="0.2">
@@ -9888,7 +9888,7 @@
         <v>21351</v>
       </c>
       <c r="AC107">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:29" x14ac:dyDescent="0.2">
@@ -9977,7 +9977,7 @@
         <v>2265</v>
       </c>
       <c r="AC108">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:29" x14ac:dyDescent="0.2">
@@ -10066,7 +10066,7 @@
         <v>91546</v>
       </c>
       <c r="AC109">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:29" x14ac:dyDescent="0.2">
@@ -10155,7 +10155,7 @@
         <v>8157</v>
       </c>
       <c r="AC110">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:29" x14ac:dyDescent="0.2">
@@ -10244,7 +10244,7 @@
         <v>4485</v>
       </c>
       <c r="AC111">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:29" x14ac:dyDescent="0.2">
@@ -10333,7 +10333,7 @@
         <v>17209</v>
       </c>
       <c r="AC112">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:29" x14ac:dyDescent="0.2">
@@ -10422,7 +10422,7 @@
         <v>7340</v>
       </c>
       <c r="AC113">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:29" x14ac:dyDescent="0.2">
@@ -10511,7 +10511,7 @@
         <v>2291</v>
       </c>
       <c r="AC114">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:29" x14ac:dyDescent="0.2">
@@ -10600,7 +10600,7 @@
         <v>7550</v>
       </c>
       <c r="AC115">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:29" x14ac:dyDescent="0.2">
@@ -10689,7 +10689,7 @@
         <v>2410</v>
       </c>
       <c r="AC116">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="1:29" x14ac:dyDescent="0.2">
@@ -10778,7 +10778,7 @@
         <v>89543</v>
       </c>
       <c r="AC117">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:29" x14ac:dyDescent="0.2">
@@ -10867,7 +10867,7 @@
         <v>8514</v>
       </c>
       <c r="AC118">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:29" x14ac:dyDescent="0.2">
@@ -10956,7 +10956,7 @@
         <v>14245</v>
       </c>
       <c r="AC119">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:29" x14ac:dyDescent="0.2">
@@ -11045,7 +11045,7 @@
         <v>42535</v>
       </c>
       <c r="AC120">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:29" x14ac:dyDescent="0.2">
@@ -11312,7 +11312,7 @@
         <v>7364</v>
       </c>
       <c r="AC123">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="124" spans="1:29" x14ac:dyDescent="0.2">
@@ -11401,7 +11401,7 @@
         <v>2079</v>
       </c>
       <c r="AC124">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="125" spans="1:29" x14ac:dyDescent="0.2">
@@ -11579,7 +11579,7 @@
         <v>31248</v>
       </c>
       <c r="AC126">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127" spans="1:29" x14ac:dyDescent="0.2">
@@ -11668,7 +11668,7 @@
         <v>26112</v>
       </c>
       <c r="AC127">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="1:29" x14ac:dyDescent="0.2">
@@ -11757,7 +11757,7 @@
         <v>9241</v>
       </c>
       <c r="AC128">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="129" spans="1:29" x14ac:dyDescent="0.2">
@@ -11935,7 +11935,7 @@
         <v>8071</v>
       </c>
       <c r="AC130">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="131" spans="1:29" x14ac:dyDescent="0.2">
@@ -12024,7 +12024,7 @@
         <v>86825</v>
       </c>
       <c r="AC131">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132" spans="1:29" x14ac:dyDescent="0.2">
@@ -12113,7 +12113,7 @@
         <v>2556</v>
       </c>
       <c r="AC132">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:29" x14ac:dyDescent="0.2">
@@ -12202,7 +12202,7 @@
         <v>56670</v>
       </c>
       <c r="AC133">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134" spans="1:29" x14ac:dyDescent="0.2">
@@ -12291,7 +12291,7 @@
         <v>2053</v>
       </c>
       <c r="AC134">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:29" x14ac:dyDescent="0.2">
@@ -12380,7 +12380,7 @@
         <v>3992</v>
       </c>
       <c r="AC135">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136" spans="1:29" x14ac:dyDescent="0.2">
@@ -12469,7 +12469,7 @@
         <v>4794</v>
       </c>
       <c r="AC136">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:29" x14ac:dyDescent="0.2">
@@ -12558,7 +12558,7 @@
         <v>13747</v>
       </c>
       <c r="AC137">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:29" x14ac:dyDescent="0.2">
@@ -12647,7 +12647,7 @@
         <v>2414</v>
       </c>
       <c r="AC138">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="139" spans="1:29" x14ac:dyDescent="0.2">
@@ -12736,7 +12736,7 @@
         <v>9322</v>
       </c>
       <c r="AC139">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140" spans="1:29" x14ac:dyDescent="0.2">
@@ -12825,7 +12825,7 @@
         <v>243762</v>
       </c>
       <c r="AC140">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:29" x14ac:dyDescent="0.2">
@@ -12914,7 +12914,7 @@
         <v>13981</v>
       </c>
       <c r="AC141">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142" spans="1:29" x14ac:dyDescent="0.2">
@@ -13003,7 +13003,7 @@
         <v>1312</v>
       </c>
       <c r="AC142">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="143" spans="1:29" x14ac:dyDescent="0.2">
@@ -13092,7 +13092,7 @@
         <v>1421345</v>
       </c>
       <c r="AC143">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="144" spans="1:29" x14ac:dyDescent="0.2">
@@ -13181,7 +13181,7 @@
         <v>1456</v>
       </c>
       <c r="AC144">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="145" spans="1:29" x14ac:dyDescent="0.2">
@@ -13359,7 +13359,7 @@
         <v>775</v>
       </c>
       <c r="AC146">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147" spans="1:29" x14ac:dyDescent="0.2">
@@ -13448,7 +13448,7 @@
         <v>2184</v>
       </c>
       <c r="AC147">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="148" spans="1:29" x14ac:dyDescent="0.2">
@@ -13537,7 +13537,7 @@
         <v>4654</v>
       </c>
       <c r="AC148">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="149" spans="1:29" x14ac:dyDescent="0.2">
@@ -13626,7 +13626,7 @@
         <v>2278</v>
       </c>
       <c r="AC149">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="150" spans="1:29" x14ac:dyDescent="0.2">
@@ -13804,7 +13804,7 @@
         <v>3868</v>
       </c>
       <c r="AC151">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="152" spans="1:29" x14ac:dyDescent="0.2">
@@ -13893,7 +13893,7 @@
         <v>7063</v>
       </c>
       <c r="AC152">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="153" spans="1:29" x14ac:dyDescent="0.2">
@@ -13982,7 +13982,7 @@
         <v>322299</v>
       </c>
       <c r="AC153">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="154" spans="1:29" x14ac:dyDescent="0.2">
@@ -14160,7 +14160,7 @@
         <v>4772</v>
       </c>
       <c r="AC155">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="156" spans="1:29" x14ac:dyDescent="0.2">
@@ -14338,7 +14338,7 @@
         <v>1388</v>
       </c>
       <c r="AC157">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158" spans="1:29" x14ac:dyDescent="0.2">
@@ -14516,7 +14516,7 @@
         <v>38798</v>
       </c>
       <c r="AC159">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="160" spans="1:29" x14ac:dyDescent="0.2">
@@ -14605,7 +14605,7 @@
         <v>1197</v>
       </c>
       <c r="AC160">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="161" spans="1:29" x14ac:dyDescent="0.2">
@@ -14694,7 +14694,7 @@
         <v>39648</v>
       </c>
       <c r="AC161">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="162" spans="1:29" x14ac:dyDescent="0.2">
@@ -14783,7 +14783,7 @@
         <v>586</v>
       </c>
       <c r="AC162">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" spans="1:29" x14ac:dyDescent="0.2">
@@ -14872,7 +14872,7 @@
         <v>862</v>
       </c>
       <c r="AC163">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="164" spans="1:29" x14ac:dyDescent="0.2">
@@ -14961,7 +14961,7 @@
         <v>1182</v>
       </c>
       <c r="AC164">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="165" spans="1:29" x14ac:dyDescent="0.2">
@@ -15228,7 +15228,7 @@
         <v>15396</v>
       </c>
       <c r="AC167">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="168" spans="1:29" x14ac:dyDescent="0.2">
@@ -15317,7 +15317,7 @@
         <v>830</v>
       </c>
       <c r="AC168">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="169" spans="1:29" x14ac:dyDescent="0.2">
@@ -15406,7 +15406,7 @@
         <v>16897</v>
       </c>
       <c r="AC169">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170" spans="1:29" x14ac:dyDescent="0.2">
@@ -15495,7 +15495,7 @@
         <v>2994</v>
       </c>
       <c r="AC170">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="171" spans="1:29" x14ac:dyDescent="0.2">
@@ -15584,7 +15584,7 @@
         <v>1719</v>
       </c>
       <c r="AC171">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="172" spans="1:29" x14ac:dyDescent="0.2">
@@ -15673,7 +15673,7 @@
         <v>696492</v>
       </c>
       <c r="AC172">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="173" spans="1:29" x14ac:dyDescent="0.2">
@@ -15762,7 +15762,7 @@
         <v>1944</v>
       </c>
       <c r="AC173">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="174" spans="1:29" x14ac:dyDescent="0.2">
@@ -15851,7 +15851,7 @@
         <v>8550</v>
       </c>
       <c r="AC174">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="175" spans="1:29" x14ac:dyDescent="0.2">
@@ -15940,7 +15940,7 @@
         <v>11584</v>
       </c>
       <c r="AC175">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="176" spans="1:29" x14ac:dyDescent="0.2">
@@ -16029,7 +16029,7 @@
         <v>2319</v>
       </c>
       <c r="AC176">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="177" spans="1:29" x14ac:dyDescent="0.2">
@@ -16118,7 +16118,7 @@
         <v>1412</v>
       </c>
       <c r="AC177">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="178" spans="1:29" x14ac:dyDescent="0.2">
@@ -16385,7 +16385,7 @@
         <v>4423</v>
       </c>
       <c r="AC180">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="181" spans="1:29" x14ac:dyDescent="0.2">
@@ -16474,7 +16474,7 @@
         <v>66142</v>
       </c>
       <c r="AC181">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="182" spans="1:29" x14ac:dyDescent="0.2">
@@ -16563,7 +16563,7 @@
         <v>16950</v>
       </c>
       <c r="AC182">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="183" spans="1:29" x14ac:dyDescent="0.2">
@@ -16652,7 +16652,7 @@
         <v>146661</v>
       </c>
       <c r="AC183">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="184" spans="1:29" x14ac:dyDescent="0.2">
@@ -16741,7 +16741,7 @@
         <v>7888</v>
       </c>
       <c r="AC184">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="185" spans="1:29" x14ac:dyDescent="0.2">
@@ -16919,7 +16919,7 @@
         <v>8143</v>
       </c>
       <c r="AC186">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="187" spans="1:29" x14ac:dyDescent="0.2">
@@ -17008,7 +17008,7 @@
         <v>2954</v>
       </c>
       <c r="AC187">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="188" spans="1:29" x14ac:dyDescent="0.2">
@@ -17097,7 +17097,7 @@
         <v>2619</v>
       </c>
       <c r="AC188">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="189" spans="1:29" x14ac:dyDescent="0.2">
@@ -17275,7 +17275,7 @@
         <v>952736</v>
       </c>
       <c r="AC190">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="191" spans="1:29" x14ac:dyDescent="0.2">
@@ -17364,7 +17364,7 @@
         <v>3974</v>
       </c>
       <c r="AC191">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="192" spans="1:29" x14ac:dyDescent="0.2">
@@ -17453,7 +17453,7 @@
         <v>24129</v>
       </c>
       <c r="AC192">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="193" spans="1:29" x14ac:dyDescent="0.2">
@@ -17631,7 +17631,7 @@
         <v>1054</v>
       </c>
       <c r="AC194">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="195" spans="1:29" x14ac:dyDescent="0.2">
@@ -17809,7 +17809,7 @@
         <v>2506</v>
       </c>
       <c r="AC196">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="197" spans="1:29" x14ac:dyDescent="0.2">
@@ -17898,7 +17898,7 @@
         <v>52500</v>
       </c>
       <c r="AC197">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="198" spans="1:29" x14ac:dyDescent="0.2">
@@ -18165,7 +18165,7 @@
         <v>1594</v>
       </c>
       <c r="AC200">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="201" spans="1:29" x14ac:dyDescent="0.2">
@@ -18254,7 +18254,7 @@
         <v>2295</v>
       </c>
       <c r="AC201">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="202" spans="1:29" x14ac:dyDescent="0.2">
@@ -18343,7 +18343,7 @@
         <v>1036</v>
       </c>
       <c r="AC202">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="203" spans="1:29" x14ac:dyDescent="0.2">
@@ -18521,7 +18521,7 @@
         <v>25389</v>
       </c>
       <c r="AC204">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="205" spans="1:29" x14ac:dyDescent="0.2">
@@ -18610,7 +18610,7 @@
         <v>35470</v>
       </c>
       <c r="AC205">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="206" spans="1:29" x14ac:dyDescent="0.2">
@@ -18699,7 +18699,7 @@
         <v>14064</v>
       </c>
       <c r="AC206">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="207" spans="1:29" x14ac:dyDescent="0.2">
@@ -18788,7 +18788,7 @@
         <v>340375</v>
       </c>
       <c r="AC207">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="208" spans="1:29" x14ac:dyDescent="0.2">
@@ -18877,7 +18877,7 @@
         <v>8090</v>
       </c>
       <c r="AC208">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="209" spans="1:29" x14ac:dyDescent="0.2">
@@ -18966,7 +18966,7 @@
         <v>694</v>
       </c>
       <c r="AC209">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="210" spans="1:29" x14ac:dyDescent="0.2">
@@ -19055,7 +19055,7 @@
         <v>137523</v>
       </c>
       <c r="AC210">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="211" spans="1:29" x14ac:dyDescent="0.2">
@@ -19144,7 +19144,7 @@
         <v>2247</v>
       </c>
       <c r="AC211">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="212" spans="1:29" x14ac:dyDescent="0.2">
@@ -19233,7 +19233,7 @@
         <v>18521</v>
       </c>
       <c r="AC212">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="213" spans="1:29" x14ac:dyDescent="0.2">
@@ -19322,7 +19322,7 @@
         <v>4831</v>
       </c>
       <c r="AC213">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="214" spans="1:29" x14ac:dyDescent="0.2">
@@ -19589,7 +19589,7 @@
         <v>241639</v>
       </c>
       <c r="AC216">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="217" spans="1:29" x14ac:dyDescent="0.2">
@@ -19767,7 +19767,7 @@
         <v>2202</v>
       </c>
       <c r="AC218">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="219" spans="1:29" x14ac:dyDescent="0.2">
@@ -19856,7 +19856,7 @@
         <v>40542</v>
       </c>
       <c r="AC219">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="220" spans="1:29" x14ac:dyDescent="0.2">
@@ -19945,7 +19945,7 @@
         <v>71547</v>
       </c>
       <c r="AC220">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="221" spans="1:29" x14ac:dyDescent="0.2">
@@ -20034,7 +20034,7 @@
         <v>1540</v>
       </c>
       <c r="AC221">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="222" spans="1:29" x14ac:dyDescent="0.2">
@@ -20123,7 +20123,7 @@
         <v>1509</v>
       </c>
       <c r="AC222">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="223" spans="1:29" x14ac:dyDescent="0.2">
@@ -20212,7 +20212,7 @@
         <v>658</v>
       </c>
       <c r="AC223">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="224" spans="1:29" x14ac:dyDescent="0.2">
@@ -20301,7 +20301,7 @@
         <v>118129</v>
       </c>
       <c r="AC224">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="225" spans="1:29" x14ac:dyDescent="0.2">
@@ -20390,7 +20390,7 @@
         <v>81915</v>
       </c>
       <c r="AC225">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="226" spans="1:29" x14ac:dyDescent="0.2">
@@ -20479,7 +20479,7 @@
         <v>20314</v>
       </c>
       <c r="AC226">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="227" spans="1:29" x14ac:dyDescent="0.2">
@@ -20568,7 +20568,7 @@
         <v>1776</v>
       </c>
       <c r="AC227">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="228" spans="1:29" x14ac:dyDescent="0.2">
@@ -20657,7 +20657,7 @@
         <v>1610</v>
       </c>
       <c r="AC228">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="229" spans="1:29" x14ac:dyDescent="0.2">
@@ -20746,7 +20746,7 @@
         <v>3730</v>
       </c>
       <c r="AC229">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="230" spans="1:29" x14ac:dyDescent="0.2">
@@ -20835,7 +20835,7 @@
         <v>1503</v>
       </c>
       <c r="AC230">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="231" spans="1:29" x14ac:dyDescent="0.2">
@@ -20924,7 +20924,7 @@
         <v>43467</v>
       </c>
       <c r="AC231">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="232" spans="1:29" x14ac:dyDescent="0.2">
@@ -21013,7 +21013,7 @@
         <v>1501</v>
       </c>
       <c r="AC232">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="233" spans="1:29" x14ac:dyDescent="0.2">
@@ -21191,7 +21191,7 @@
         <v>400</v>
       </c>
       <c r="AC234">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="235" spans="1:29" x14ac:dyDescent="0.2">
@@ -21280,7 +21280,7 @@
         <v>6402</v>
       </c>
       <c r="AC235">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="236" spans="1:29" x14ac:dyDescent="0.2">
@@ -21369,7 +21369,7 @@
         <v>1859</v>
       </c>
       <c r="AC236">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="237" spans="1:29" x14ac:dyDescent="0.2">
@@ -21458,7 +21458,7 @@
         <v>1117</v>
       </c>
       <c r="AC237">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="238" spans="1:29" x14ac:dyDescent="0.2">
@@ -21547,7 +21547,7 @@
         <v>152464</v>
       </c>
       <c r="AC238">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="239" spans="1:29" x14ac:dyDescent="0.2">
@@ -21636,7 +21636,7 @@
         <v>135995</v>
       </c>
       <c r="AC239">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="240" spans="1:29" x14ac:dyDescent="0.2">
@@ -21725,7 +21725,7 @@
         <v>10168</v>
       </c>
       <c r="AC240">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="241" spans="1:29" x14ac:dyDescent="0.2">
@@ -21814,7 +21814,7 @@
         <v>1607</v>
       </c>
       <c r="AC241">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="242" spans="1:29" x14ac:dyDescent="0.2">
@@ -21903,7 +21903,7 @@
         <v>10925</v>
       </c>
       <c r="AC242">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="243" spans="1:29" x14ac:dyDescent="0.2">
@@ -21992,7 +21992,7 @@
         <v>17852</v>
       </c>
       <c r="AC243">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="244" spans="1:29" x14ac:dyDescent="0.2">
@@ -22081,7 +22081,7 @@
         <v>4769</v>
       </c>
       <c r="AC244">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="245" spans="1:29" x14ac:dyDescent="0.2">
@@ -22170,7 +22170,7 @@
         <v>51702</v>
       </c>
       <c r="AC245">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="246" spans="1:29" x14ac:dyDescent="0.2">
@@ -22259,7 +22259,7 @@
         <v>6934</v>
       </c>
       <c r="AC246">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="247" spans="1:29" x14ac:dyDescent="0.2">
@@ -22348,7 +22348,7 @@
         <v>7328</v>
       </c>
       <c r="AC247">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="248" spans="1:29" x14ac:dyDescent="0.2">
@@ -22437,7 +22437,7 @@
         <v>14509</v>
       </c>
       <c r="AC248">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="249" spans="1:29" x14ac:dyDescent="0.2">
@@ -22526,7 +22526,7 @@
         <v>44911</v>
       </c>
       <c r="AC249">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="250" spans="1:29" x14ac:dyDescent="0.2">
@@ -22615,7 +22615,7 @@
         <v>1689</v>
       </c>
       <c r="AC250">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="251" spans="1:29" x14ac:dyDescent="0.2">
@@ -22704,7 +22704,7 @@
         <v>20846</v>
       </c>
       <c r="AC251">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="252" spans="1:29" x14ac:dyDescent="0.2">
@@ -22882,7 +22882,7 @@
         <v>10693</v>
       </c>
       <c r="AC253">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="254" spans="1:29" x14ac:dyDescent="0.2">
@@ -22971,7 +22971,7 @@
         <v>20221</v>
       </c>
       <c r="AC254">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="255" spans="1:29" x14ac:dyDescent="0.2">
@@ -23149,7 +23149,7 @@
         <v>9722</v>
       </c>
       <c r="AC256">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="257" spans="1:29" x14ac:dyDescent="0.2">
@@ -23327,7 +23327,7 @@
         <v>11835</v>
       </c>
       <c r="AC258">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="259" spans="1:29" x14ac:dyDescent="0.2">
@@ -23416,7 +23416,7 @@
         <v>62670</v>
       </c>
       <c r="AC259">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="260" spans="1:29" x14ac:dyDescent="0.2">
@@ -23505,7 +23505,7 @@
         <v>1583</v>
       </c>
       <c r="AC260">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="261" spans="1:29" x14ac:dyDescent="0.2">
@@ -23683,7 +23683,7 @@
         <v>49465</v>
       </c>
       <c r="AC262">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="263" spans="1:29" x14ac:dyDescent="0.2">
@@ -23772,7 +23772,7 @@
         <v>48217</v>
       </c>
       <c r="AC263">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="264" spans="1:29" x14ac:dyDescent="0.2">
@@ -24039,7 +24039,7 @@
         <v>2106</v>
       </c>
       <c r="AC266">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="267" spans="1:29" x14ac:dyDescent="0.2">
@@ -24128,7 +24128,7 @@
         <v>6388</v>
       </c>
       <c r="AC267">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="268" spans="1:29" x14ac:dyDescent="0.2">
@@ -24217,7 +24217,7 @@
         <v>963</v>
       </c>
       <c r="AC268">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="269" spans="1:29" x14ac:dyDescent="0.2">
@@ -24306,7 +24306,7 @@
         <v>6710</v>
       </c>
       <c r="AC269">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="270" spans="1:29" x14ac:dyDescent="0.2">
@@ -24395,7 +24395,7 @@
         <v>1069</v>
       </c>
       <c r="AC270">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="271" spans="1:29" x14ac:dyDescent="0.2">
@@ -24484,7 +24484,7 @@
         <v>3257</v>
       </c>
       <c r="AC271">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="272" spans="1:29" x14ac:dyDescent="0.2">
@@ -24662,7 +24662,7 @@
         <v>11163</v>
       </c>
       <c r="AC273">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="274" spans="1:29" x14ac:dyDescent="0.2">
@@ -24751,7 +24751,7 @@
         <v>14650</v>
       </c>
       <c r="AC274">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="275" spans="1:29" x14ac:dyDescent="0.2">
@@ -24840,7 +24840,7 @@
         <v>1601129</v>
       </c>
       <c r="AC275">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="276" spans="1:29" x14ac:dyDescent="0.2">
@@ -24929,7 +24929,7 @@
         <v>917776</v>
       </c>
       <c r="AC276">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="277" spans="1:29" x14ac:dyDescent="0.2">
@@ -25018,7 +25018,7 @@
         <v>6215</v>
       </c>
       <c r="AC277">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="278" spans="1:29" x14ac:dyDescent="0.2">
@@ -25107,7 +25107,7 @@
         <v>11896</v>
       </c>
       <c r="AC278">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="279" spans="1:29" x14ac:dyDescent="0.2">
@@ -25196,7 +25196,7 @@
         <v>1124668</v>
       </c>
       <c r="AC279">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="280" spans="1:29" x14ac:dyDescent="0.2">
@@ -25285,7 +25285,7 @@
         <v>246852</v>
       </c>
       <c r="AC280">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="281" spans="1:29" x14ac:dyDescent="0.2">
@@ -25374,7 +25374,7 @@
         <v>3333</v>
       </c>
       <c r="AC281">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="282" spans="1:29" x14ac:dyDescent="0.2">
@@ -25463,7 +25463,7 @@
         <v>7890</v>
       </c>
       <c r="AC282">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="283" spans="1:29" x14ac:dyDescent="0.2">
@@ -25552,7 +25552,7 @@
         <v>2022964</v>
       </c>
       <c r="AC283">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="284" spans="1:29" x14ac:dyDescent="0.2">
@@ -25641,7 +25641,7 @@
         <v>104689</v>
       </c>
       <c r="AC284">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="285" spans="1:29" x14ac:dyDescent="0.2">
@@ -25730,7 +25730,7 @@
         <v>88316</v>
       </c>
       <c r="AC285">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="286" spans="1:29" x14ac:dyDescent="0.2">
@@ -25819,7 +25819,7 @@
         <v>48809</v>
       </c>
       <c r="AC286">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="287" spans="1:29" x14ac:dyDescent="0.2">
@@ -25997,7 +25997,7 @@
         <v>48562</v>
       </c>
       <c r="AC288">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="289" spans="1:29" x14ac:dyDescent="0.2">
@@ -26086,7 +26086,7 @@
         <v>1243</v>
       </c>
       <c r="AC289">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="290" spans="1:29" x14ac:dyDescent="0.2">
@@ -26175,7 +26175,7 @@
         <v>11320</v>
       </c>
       <c r="AC290">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="291" spans="1:29" x14ac:dyDescent="0.2">
@@ -26264,7 +26264,7 @@
         <v>634</v>
       </c>
       <c r="AC291">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="292" spans="1:29" x14ac:dyDescent="0.2">
@@ -26353,7 +26353,7 @@
         <v>3852</v>
       </c>
       <c r="AC292">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="293" spans="1:29" x14ac:dyDescent="0.2">
@@ -26442,7 +26442,7 @@
         <v>774730</v>
       </c>
       <c r="AC293">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="294" spans="1:29" x14ac:dyDescent="0.2">
@@ -26531,7 +26531,7 @@
         <v>2537</v>
       </c>
       <c r="AC294">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="295" spans="1:29" x14ac:dyDescent="0.2">
@@ -26620,7 +26620,7 @@
         <v>3601</v>
       </c>
       <c r="AC295">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="296" spans="1:29" x14ac:dyDescent="0.2">
@@ -26798,7 +26798,7 @@
         <v>1256</v>
       </c>
       <c r="AC297">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="298" spans="1:29" x14ac:dyDescent="0.2">
@@ -26887,7 +26887,7 @@
         <v>9049</v>
       </c>
       <c r="AC298">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="299" spans="1:29" x14ac:dyDescent="0.2">
@@ -26976,7 +26976,7 @@
         <v>9455</v>
       </c>
       <c r="AC299">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="300" spans="1:29" x14ac:dyDescent="0.2">
@@ -27065,7 +27065,7 @@
         <v>1383</v>
       </c>
       <c r="AC300">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="301" spans="1:29" x14ac:dyDescent="0.2">
@@ -27154,7 +27154,7 @@
         <v>1293111</v>
       </c>
       <c r="AC301">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="302" spans="1:29" x14ac:dyDescent="0.2">
@@ -27243,7 +27243,7 @@
         <v>2671</v>
       </c>
       <c r="AC302">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="303" spans="1:29" x14ac:dyDescent="0.2">
@@ -27332,7 +27332,7 @@
         <v>7696</v>
       </c>
       <c r="AC303">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="304" spans="1:29" x14ac:dyDescent="0.2">
@@ -27421,7 +27421,7 @@
         <v>3623</v>
       </c>
       <c r="AC304">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="305" spans="1:29" x14ac:dyDescent="0.2">
@@ -27510,7 +27510,7 @@
         <v>42021</v>
       </c>
       <c r="AC305">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="306" spans="1:29" x14ac:dyDescent="0.2">
@@ -27599,7 +27599,7 @@
         <v>5477</v>
       </c>
       <c r="AC306">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="307" spans="1:29" x14ac:dyDescent="0.2">
@@ -27688,7 +27688,7 @@
         <v>51588</v>
       </c>
       <c r="AC307">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="308" spans="1:29" x14ac:dyDescent="0.2">
@@ -27777,7 +27777,7 @@
         <v>6432</v>
       </c>
       <c r="AC308">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="309" spans="1:29" x14ac:dyDescent="0.2">
@@ -27866,7 +27866,7 @@
         <v>41955</v>
       </c>
       <c r="AC309">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="310" spans="1:29" x14ac:dyDescent="0.2">
@@ -27955,7 +27955,7 @@
         <v>5367</v>
       </c>
       <c r="AC310">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="311" spans="1:29" x14ac:dyDescent="0.2">
@@ -28044,7 +28044,7 @@
         <v>2472</v>
       </c>
       <c r="AC311">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="312" spans="1:29" x14ac:dyDescent="0.2">
@@ -28133,7 +28133,7 @@
         <v>12072</v>
       </c>
       <c r="AC312">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="313" spans="1:29" x14ac:dyDescent="0.2">
@@ -28222,7 +28222,7 @@
         <v>19738</v>
       </c>
       <c r="AC313">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="314" spans="1:29" x14ac:dyDescent="0.2">
@@ -28311,7 +28311,7 @@
         <v>2798</v>
       </c>
       <c r="AC314">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="315" spans="1:29" x14ac:dyDescent="0.2">
@@ -28400,7 +28400,7 @@
         <v>920</v>
       </c>
       <c r="AC315">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="316" spans="1:29" x14ac:dyDescent="0.2">
@@ -28578,7 +28578,7 @@
         <v>3273</v>
       </c>
       <c r="AC317">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="318" spans="1:29" x14ac:dyDescent="0.2">
@@ -28667,7 +28667,7 @@
         <v>3051</v>
       </c>
       <c r="AC318">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="319" spans="1:29" x14ac:dyDescent="0.2">
@@ -28756,7 +28756,7 @@
         <v>1126</v>
       </c>
       <c r="AC319">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="320" spans="1:29" x14ac:dyDescent="0.2">
@@ -28845,7 +28845,7 @@
         <v>5167</v>
       </c>
       <c r="AC320">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="321" spans="1:29" x14ac:dyDescent="0.2">
@@ -28934,7 +28934,7 @@
         <v>466769</v>
       </c>
       <c r="AC321">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="322" spans="1:29" x14ac:dyDescent="0.2">
@@ -29023,7 +29023,7 @@
         <v>2517</v>
       </c>
       <c r="AC322">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="323" spans="1:29" x14ac:dyDescent="0.2">
@@ -29112,7 +29112,7 @@
         <v>5073</v>
       </c>
       <c r="AC323">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="324" spans="1:29" x14ac:dyDescent="0.2">
@@ -29201,7 +29201,7 @@
         <v>762590</v>
       </c>
       <c r="AC324">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="325" spans="1:29" x14ac:dyDescent="0.2">
@@ -29290,7 +29290,7 @@
         <v>1635</v>
       </c>
       <c r="AC325">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="326" spans="1:29" x14ac:dyDescent="0.2">
@@ -29379,7 +29379,7 @@
         <v>10746</v>
       </c>
       <c r="AC326">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="327" spans="1:29" x14ac:dyDescent="0.2">
@@ -29468,7 +29468,7 @@
         <v>1702</v>
       </c>
       <c r="AC327">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="328" spans="1:29" x14ac:dyDescent="0.2">
@@ -29557,7 +29557,7 @@
         <v>9720</v>
       </c>
       <c r="AC328">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="329" spans="1:29" x14ac:dyDescent="0.2">
@@ -29646,7 +29646,7 @@
         <v>1563</v>
       </c>
       <c r="AC329">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="330" spans="1:29" x14ac:dyDescent="0.2">
@@ -29735,7 +29735,7 @@
         <v>15154</v>
       </c>
       <c r="AC330">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="331" spans="1:29" x14ac:dyDescent="0.2">
@@ -29824,7 +29824,7 @@
         <v>312397</v>
       </c>
       <c r="AC331">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="332" spans="1:29" x14ac:dyDescent="0.2">
@@ -29913,7 +29913,7 @@
         <v>2118</v>
       </c>
       <c r="AC332">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="333" spans="1:29" x14ac:dyDescent="0.2">
@@ -30002,7 +30002,7 @@
         <v>68948</v>
       </c>
       <c r="AC333">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="334" spans="1:29" x14ac:dyDescent="0.2">
@@ -30091,7 +30091,7 @@
         <v>36368</v>
       </c>
       <c r="AC334">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="335" spans="1:29" x14ac:dyDescent="0.2">
@@ -30180,7 +30180,7 @@
         <v>17669</v>
       </c>
       <c r="AC335">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="336" spans="1:29" x14ac:dyDescent="0.2">
@@ -30358,7 +30358,7 @@
         <v>3264</v>
       </c>
       <c r="AC337">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="338" spans="1:29" x14ac:dyDescent="0.2">
@@ -30447,7 +30447,7 @@
         <v>13796</v>
       </c>
       <c r="AC338">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="339" spans="1:29" x14ac:dyDescent="0.2">
@@ -30536,7 +30536,7 @@
         <v>97513</v>
       </c>
       <c r="AC339">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="340" spans="1:29" x14ac:dyDescent="0.2">
@@ -30625,7 +30625,7 @@
         <v>2353</v>
       </c>
       <c r="AC340">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="341" spans="1:29" x14ac:dyDescent="0.2">
@@ -30714,7 +30714,7 @@
         <v>23216</v>
       </c>
       <c r="AC341">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>